<commit_message>
preparing for peer review
</commit_message>
<xml_diff>
--- a/coxregression.xlsx
+++ b/coxregression.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenggu\University of Michigan Dropbox\Feng Gu\GitHub\MachineLearningOnHFData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3B2FA2-7412-4462-A581-6DC7197C540C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E684E43-B54B-468F-802B-B1FCC3523708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1305" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>PCWP_D</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Cardiomyopathy</t>
-  </si>
-  <si>
-    <t>Septal E/E'</t>
   </si>
   <si>
     <t>BNP</t>
@@ -248,6 +245,12 @@
   <si>
     <t>MVr_D</t>
   </si>
+  <si>
+    <t>MAGGIC</t>
+  </si>
+  <si>
+    <t>Septal_Eprime</t>
+  </si>
 </sst>
 </file>
 
@@ -297,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -309,6 +312,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BV347"/>
+  <dimension ref="A1:BW347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BL1" sqref="BL1:BL1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +629,7 @@
     <col min="59" max="63" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -673,13 +679,13 @@
         <v>17</v>
       </c>
       <c r="Q1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>14</v>
@@ -688,166 +694,169 @@
         <v>15</v>
       </c>
       <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AC1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AE1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AS1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BJ1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BK1" t="s">
         <v>56</v>
       </c>
-      <c r="AT1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BF1" t="s">
+      <c r="BL1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="BG1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BJ1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BL1" s="5" t="s">
+      <c r="BM1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="5" t="s">
+      <c r="BN1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="5" t="s">
+      <c r="BO1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="5" t="s">
+      <c r="BP1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" s="5" t="s">
+      <c r="BQ1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BR1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" s="5" t="s">
+      <c r="BS1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" s="5" t="s">
+      <c r="BT1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" s="5" t="s">
+      <c r="BU1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" s="5" t="s">
+      <c r="BV1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" s="5" t="s">
-        <v>72</v>
+      <c r="BW1" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1070,8 +1079,11 @@
       <c r="BV2" s="4">
         <v>0</v>
       </c>
+      <c r="BW2" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>26</v>
       </c>
@@ -1294,8 +1306,11 @@
       <c r="BV3" s="4">
         <v>1</v>
       </c>
+      <c r="BW3" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1518,8 +1533,11 @@
       <c r="BV4" s="4">
         <v>0</v>
       </c>
+      <c r="BW4" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>33</v>
       </c>
@@ -1742,8 +1760,11 @@
       <c r="BV5" s="4">
         <v>1</v>
       </c>
+      <c r="BW5" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>18</v>
       </c>
@@ -1966,8 +1987,11 @@
       <c r="BV6" s="4">
         <v>0</v>
       </c>
+      <c r="BW6" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>22</v>
       </c>
@@ -2190,8 +2214,11 @@
       <c r="BV7" s="4">
         <v>1</v>
       </c>
+      <c r="BW7" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -2414,8 +2441,11 @@
       <c r="BV8" s="4">
         <v>0</v>
       </c>
+      <c r="BW8" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>24</v>
       </c>
@@ -2638,8 +2668,11 @@
       <c r="BV9" s="4">
         <v>1</v>
       </c>
+      <c r="BW9" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="10" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -2862,8 +2895,11 @@
       <c r="BV10" s="4">
         <v>0</v>
       </c>
+      <c r="BW10" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>24</v>
       </c>
@@ -3086,8 +3122,11 @@
       <c r="BV11" s="4">
         <v>0</v>
       </c>
+      <c r="BW11" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>18</v>
       </c>
@@ -3310,8 +3349,11 @@
       <c r="BV12" s="4">
         <v>0</v>
       </c>
+      <c r="BW12" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -3534,8 +3576,11 @@
       <c r="BV13" s="4">
         <v>0</v>
       </c>
+      <c r="BW13" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>16</v>
       </c>
@@ -3758,8 +3803,11 @@
       <c r="BV14" s="4">
         <v>0</v>
       </c>
+      <c r="BW14" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>19</v>
       </c>
@@ -3982,8 +4030,11 @@
       <c r="BV15" s="4">
         <v>0</v>
       </c>
+      <c r="BW15" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -4206,8 +4257,11 @@
       <c r="BV16" s="4">
         <v>0</v>
       </c>
+      <c r="BW16" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="17" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4430,8 +4484,11 @@
       <c r="BV17" s="4">
         <v>0</v>
       </c>
+      <c r="BW17" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="18" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -4654,8 +4711,11 @@
       <c r="BV18" s="4">
         <v>0</v>
       </c>
+      <c r="BW18" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="19" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4878,8 +4938,11 @@
       <c r="BV19" s="4">
         <v>1</v>
       </c>
+      <c r="BW19" s="6">
+        <v>26</v>
+      </c>
     </row>
-    <row r="20" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -5102,8 +5165,11 @@
       <c r="BV20" s="4">
         <v>0</v>
       </c>
+      <c r="BW20" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="21" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5326,8 +5392,11 @@
       <c r="BV21" s="4">
         <v>1</v>
       </c>
+      <c r="BW21" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="22" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
@@ -5550,8 +5619,11 @@
       <c r="BV22" s="4">
         <v>1</v>
       </c>
+      <c r="BW22" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="23" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5774,8 +5846,11 @@
       <c r="BV23" s="4">
         <v>0</v>
       </c>
+      <c r="BW23" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="24" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -5998,8 +6073,11 @@
       <c r="BV24" s="4">
         <v>0</v>
       </c>
+      <c r="BW24" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="25" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>14</v>
       </c>
@@ -6222,8 +6300,11 @@
       <c r="BV25" s="4">
         <v>1</v>
       </c>
+      <c r="BW25" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="26" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6446,8 +6527,11 @@
       <c r="BV26" s="4">
         <v>0</v>
       </c>
+      <c r="BW26" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="27" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>17</v>
       </c>
@@ -6670,8 +6754,11 @@
       <c r="BV27" s="4">
         <v>1</v>
       </c>
+      <c r="BW27" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="28" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -6894,8 +6981,11 @@
       <c r="BV28" s="4">
         <v>0</v>
       </c>
+      <c r="BW28" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="29" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>24</v>
       </c>
@@ -7118,8 +7208,11 @@
       <c r="BV29" s="4">
         <v>1</v>
       </c>
+      <c r="BW29" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="30" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>34</v>
       </c>
@@ -7342,8 +7435,11 @@
       <c r="BV30" s="4">
         <v>1</v>
       </c>
+      <c r="BW30" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="31" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>23</v>
       </c>
@@ -7566,8 +7662,11 @@
       <c r="BV31" s="4">
         <v>1</v>
       </c>
+      <c r="BW31" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="32" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>23</v>
       </c>
@@ -7790,8 +7889,11 @@
       <c r="BV32" s="4">
         <v>1</v>
       </c>
+      <c r="BW32" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="33" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>26</v>
       </c>
@@ -8014,8 +8116,11 @@
       <c r="BV33" s="4">
         <v>1</v>
       </c>
+      <c r="BW33" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="34" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>38</v>
       </c>
@@ -8238,8 +8343,11 @@
       <c r="BV34" s="4">
         <v>1</v>
       </c>
+      <c r="BW34" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="35" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>16</v>
       </c>
@@ -8462,8 +8570,11 @@
       <c r="BV35" s="4">
         <v>0</v>
       </c>
+      <c r="BW35" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="36" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
@@ -8686,8 +8797,11 @@
       <c r="BV36" s="4">
         <v>1</v>
       </c>
+      <c r="BW36" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="37" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>25</v>
       </c>
@@ -8910,8 +9024,11 @@
       <c r="BV37" s="4">
         <v>0</v>
       </c>
+      <c r="BW37" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="38" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>13</v>
       </c>
@@ -9134,8 +9251,11 @@
       <c r="BV38" s="4">
         <v>1</v>
       </c>
+      <c r="BW38" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="39" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>19</v>
       </c>
@@ -9358,8 +9478,11 @@
       <c r="BV39" s="4">
         <v>1</v>
       </c>
+      <c r="BW39" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="40" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>24</v>
       </c>
@@ -9582,8 +9705,11 @@
       <c r="BV40" s="4">
         <v>1</v>
       </c>
+      <c r="BW40" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="41" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>20</v>
       </c>
@@ -9806,8 +9932,11 @@
       <c r="BV41" s="4">
         <v>0</v>
       </c>
+      <c r="BW41" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="42" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>20</v>
       </c>
@@ -10030,8 +10159,11 @@
       <c r="BV42" s="4">
         <v>0</v>
       </c>
+      <c r="BW42" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="43" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>23</v>
       </c>
@@ -10254,8 +10386,11 @@
       <c r="BV43" s="4">
         <v>1</v>
       </c>
+      <c r="BW43" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="44" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>24</v>
       </c>
@@ -10478,8 +10613,11 @@
       <c r="BV44" s="4">
         <v>0</v>
       </c>
+      <c r="BW44" s="6">
+        <v>34</v>
+      </c>
     </row>
-    <row r="45" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>18</v>
       </c>
@@ -10702,8 +10840,11 @@
       <c r="BV45" s="4">
         <v>0</v>
       </c>
+      <c r="BW45" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="46" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>12</v>
       </c>
@@ -10926,8 +11067,11 @@
       <c r="BV46" s="4">
         <v>1</v>
       </c>
+      <c r="BW46" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="47" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>12</v>
       </c>
@@ -11150,8 +11294,11 @@
       <c r="BV47" s="4">
         <v>1</v>
       </c>
+      <c r="BW47" s="6">
+        <v>25</v>
+      </c>
     </row>
-    <row r="48" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20</v>
       </c>
@@ -11374,8 +11521,11 @@
       <c r="BV48" s="4">
         <v>0</v>
       </c>
+      <c r="BW48" s="6">
+        <v>26</v>
+      </c>
     </row>
-    <row r="49" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>11</v>
       </c>
@@ -11598,8 +11748,11 @@
       <c r="BV49" s="4">
         <v>0</v>
       </c>
+      <c r="BW49" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="50" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>31</v>
       </c>
@@ -11822,8 +11975,11 @@
       <c r="BV50" s="4">
         <v>1</v>
       </c>
+      <c r="BW50" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="51" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>11</v>
       </c>
@@ -12046,8 +12202,11 @@
       <c r="BV51" s="4">
         <v>0</v>
       </c>
+      <c r="BW51" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="52" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>25</v>
       </c>
@@ -12270,8 +12429,11 @@
       <c r="BV52" s="4">
         <v>1</v>
       </c>
+      <c r="BW52" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="53" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>22</v>
       </c>
@@ -12494,8 +12656,11 @@
       <c r="BV53" s="4">
         <v>1</v>
       </c>
+      <c r="BW53" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="54" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>19</v>
       </c>
@@ -12718,8 +12883,11 @@
       <c r="BV54" s="4">
         <v>1</v>
       </c>
+      <c r="BW54" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="55" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>13</v>
       </c>
@@ -12942,8 +13110,11 @@
       <c r="BV55" s="4">
         <v>0</v>
       </c>
+      <c r="BW55" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="56" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>12</v>
       </c>
@@ -13166,8 +13337,11 @@
       <c r="BV56" s="4">
         <v>0</v>
       </c>
+      <c r="BW56" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="57" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>12</v>
       </c>
@@ -13390,8 +13564,11 @@
       <c r="BV57" s="4">
         <v>1</v>
       </c>
+      <c r="BW57" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="58" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>24</v>
       </c>
@@ -13614,8 +13791,11 @@
       <c r="BV58" s="4">
         <v>1</v>
       </c>
+      <c r="BW58" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="59" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4</v>
       </c>
@@ -13838,8 +14018,11 @@
       <c r="BV59" s="4">
         <v>0</v>
       </c>
+      <c r="BW59" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="60" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>18</v>
       </c>
@@ -14062,8 +14245,11 @@
       <c r="BV60" s="4">
         <v>0</v>
       </c>
+      <c r="BW60" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="61" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>13</v>
       </c>
@@ -14286,8 +14472,11 @@
       <c r="BV61" s="4">
         <v>0</v>
       </c>
+      <c r="BW61" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="62" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>18</v>
       </c>
@@ -14510,8 +14699,11 @@
       <c r="BV62" s="4">
         <v>0</v>
       </c>
+      <c r="BW62" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="63" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>14</v>
       </c>
@@ -14734,8 +14926,11 @@
       <c r="BV63" s="4">
         <v>0</v>
       </c>
+      <c r="BW63" s="6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="64" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>39</v>
       </c>
@@ -14958,8 +15153,11 @@
       <c r="BV64" s="4">
         <v>0</v>
       </c>
+      <c r="BW64" s="6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="65" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>15</v>
       </c>
@@ -15182,8 +15380,11 @@
       <c r="BV65" s="4">
         <v>0</v>
       </c>
+      <c r="BW65" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="66" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>15</v>
       </c>
@@ -15406,8 +15607,11 @@
       <c r="BV66" s="4">
         <v>1</v>
       </c>
+      <c r="BW66" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="67" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>14</v>
       </c>
@@ -15630,8 +15834,11 @@
       <c r="BV67" s="4">
         <v>1</v>
       </c>
+      <c r="BW67" s="6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="68" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>19</v>
       </c>
@@ -15854,8 +16061,11 @@
       <c r="BV68" s="4">
         <v>0</v>
       </c>
+      <c r="BW68" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="69" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>8</v>
       </c>
@@ -16078,8 +16288,11 @@
       <c r="BV69" s="4">
         <v>0</v>
       </c>
+      <c r="BW69" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="70" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9</v>
       </c>
@@ -16302,8 +16515,11 @@
       <c r="BV70" s="4">
         <v>0</v>
       </c>
+      <c r="BW70" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="71" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>21</v>
       </c>
@@ -16526,8 +16742,11 @@
       <c r="BV71" s="4">
         <v>1</v>
       </c>
+      <c r="BW71" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="72" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>19</v>
       </c>
@@ -16750,8 +16969,11 @@
       <c r="BV72" s="4">
         <v>0</v>
       </c>
+      <c r="BW72" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="73" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>7</v>
       </c>
@@ -16974,8 +17196,11 @@
       <c r="BV73" s="4">
         <v>0</v>
       </c>
+      <c r="BW73" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="74" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>8</v>
       </c>
@@ -17198,8 +17423,11 @@
       <c r="BV74" s="4">
         <v>0</v>
       </c>
+      <c r="BW74" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="75" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>23</v>
       </c>
@@ -17422,8 +17650,11 @@
       <c r="BV75" s="4">
         <v>0</v>
       </c>
+      <c r="BW75" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="76" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>19</v>
       </c>
@@ -17646,8 +17877,11 @@
       <c r="BV76" s="4">
         <v>0</v>
       </c>
+      <c r="BW76" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="77" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>34</v>
       </c>
@@ -17870,8 +18104,11 @@
       <c r="BV77" s="4">
         <v>1</v>
       </c>
+      <c r="BW77" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="78" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>25</v>
       </c>
@@ -18094,8 +18331,11 @@
       <c r="BV78" s="4">
         <v>1</v>
       </c>
+      <c r="BW78" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="79" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>29</v>
       </c>
@@ -18318,8 +18558,11 @@
       <c r="BV79" s="4">
         <v>0</v>
       </c>
+      <c r="BW79" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="80" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>9</v>
       </c>
@@ -18542,8 +18785,11 @@
       <c r="BV80" s="4">
         <v>1</v>
       </c>
+      <c r="BW80" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="81" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>9</v>
       </c>
@@ -18766,8 +19012,11 @@
       <c r="BV81" s="4">
         <v>1</v>
       </c>
+      <c r="BW81" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="82" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>10</v>
       </c>
@@ -18990,8 +19239,11 @@
       <c r="BV82" s="4">
         <v>0</v>
       </c>
+      <c r="BW82" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="83" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>7</v>
       </c>
@@ -19214,8 +19466,11 @@
       <c r="BV83" s="4">
         <v>1</v>
       </c>
+      <c r="BW83" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="84" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>10</v>
       </c>
@@ -19438,8 +19693,11 @@
       <c r="BV84" s="4">
         <v>0</v>
       </c>
+      <c r="BW84" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="85" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>18</v>
       </c>
@@ -19662,8 +19920,11 @@
       <c r="BV85" s="4">
         <v>1</v>
       </c>
+      <c r="BW85" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="86" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>6</v>
       </c>
@@ -19886,8 +20147,11 @@
       <c r="BV86" s="4">
         <v>0</v>
       </c>
+      <c r="BW86" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="87" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>8</v>
       </c>
@@ -20110,8 +20374,11 @@
       <c r="BV87" s="4">
         <v>1</v>
       </c>
+      <c r="BW87" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="88" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>42</v>
       </c>
@@ -20334,8 +20601,11 @@
       <c r="BV88" s="4">
         <v>1</v>
       </c>
+      <c r="BW88" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="89" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>22</v>
       </c>
@@ -20558,8 +20828,11 @@
       <c r="BV89" s="4">
         <v>0</v>
       </c>
+      <c r="BW89" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="90" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>13</v>
       </c>
@@ -20782,8 +21055,11 @@
       <c r="BV90" s="4">
         <v>0</v>
       </c>
+      <c r="BW90" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="91" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>21</v>
       </c>
@@ -21006,8 +21282,11 @@
       <c r="BV91" s="4">
         <v>0</v>
       </c>
+      <c r="BW91" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="92" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>18</v>
       </c>
@@ -21230,8 +21509,11 @@
       <c r="BV92" s="4">
         <v>1</v>
       </c>
+      <c r="BW92" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="93" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>19</v>
       </c>
@@ -21454,8 +21736,11 @@
       <c r="BV93" s="4">
         <v>0</v>
       </c>
+      <c r="BW93" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="94" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>13</v>
       </c>
@@ -21678,8 +21963,11 @@
       <c r="BV94" s="4">
         <v>1</v>
       </c>
+      <c r="BW94" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="95" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>22</v>
       </c>
@@ -21902,8 +22190,11 @@
       <c r="BV95" s="4">
         <v>0</v>
       </c>
+      <c r="BW95" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="96" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>17</v>
       </c>
@@ -22126,8 +22417,11 @@
       <c r="BV96" s="4">
         <v>0</v>
       </c>
+      <c r="BW96" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="97" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>9</v>
       </c>
@@ -22350,8 +22644,11 @@
       <c r="BV97" s="4">
         <v>1</v>
       </c>
+      <c r="BW97" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="98" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>25</v>
       </c>
@@ -22574,8 +22871,11 @@
       <c r="BV98" s="4">
         <v>0</v>
       </c>
+      <c r="BW98" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="99" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>12</v>
       </c>
@@ -22798,8 +23098,11 @@
       <c r="BV99" s="4">
         <v>0</v>
       </c>
+      <c r="BW99" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="100" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>13</v>
       </c>
@@ -23022,8 +23325,11 @@
       <c r="BV100" s="4">
         <v>0</v>
       </c>
+      <c r="BW100" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="101" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>14</v>
       </c>
@@ -23246,8 +23552,11 @@
       <c r="BV101" s="4">
         <v>0</v>
       </c>
+      <c r="BW101" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="102" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>24</v>
       </c>
@@ -23470,8 +23779,11 @@
       <c r="BV102" s="4">
         <v>1</v>
       </c>
+      <c r="BW102" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="103" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>15</v>
       </c>
@@ -23694,8 +24006,11 @@
       <c r="BV103" s="4">
         <v>0</v>
       </c>
+      <c r="BW103" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="104" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>25</v>
       </c>
@@ -23918,8 +24233,11 @@
       <c r="BV104" s="4">
         <v>0</v>
       </c>
+      <c r="BW104" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="105" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>31</v>
       </c>
@@ -24142,8 +24460,11 @@
       <c r="BV105" s="4">
         <v>0</v>
       </c>
+      <c r="BW105" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="106" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>18</v>
       </c>
@@ -24366,8 +24687,11 @@
       <c r="BV106" s="4">
         <v>1</v>
       </c>
+      <c r="BW106" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="107" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>23</v>
       </c>
@@ -24590,8 +24914,11 @@
       <c r="BV107" s="4">
         <v>0</v>
       </c>
+      <c r="BW107" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="108" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>12</v>
       </c>
@@ -24814,8 +25141,11 @@
       <c r="BV108" s="4">
         <v>0</v>
       </c>
+      <c r="BW108" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="109" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>14</v>
       </c>
@@ -25038,8 +25368,11 @@
       <c r="BV109" s="4">
         <v>0</v>
       </c>
+      <c r="BW109" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="110" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>13</v>
       </c>
@@ -25262,8 +25595,11 @@
       <c r="BV110" s="4">
         <v>0</v>
       </c>
+      <c r="BW110" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="111" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>24</v>
       </c>
@@ -25486,8 +25822,11 @@
       <c r="BV111" s="4">
         <v>0</v>
       </c>
+      <c r="BW111" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="112" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>12</v>
       </c>
@@ -25710,8 +26049,11 @@
       <c r="BV112" s="4">
         <v>0</v>
       </c>
+      <c r="BW112" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="113" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>25</v>
       </c>
@@ -25934,8 +26276,11 @@
       <c r="BV113" s="4">
         <v>0</v>
       </c>
+      <c r="BW113" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="114" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>8</v>
       </c>
@@ -26158,8 +26503,11 @@
       <c r="BV114" s="4">
         <v>1</v>
       </c>
+      <c r="BW114" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="115" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>18</v>
       </c>
@@ -26382,8 +26730,11 @@
       <c r="BV115" s="4">
         <v>0</v>
       </c>
+      <c r="BW115" s="6">
+        <v>27</v>
+      </c>
     </row>
-    <row r="116" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>14</v>
       </c>
@@ -26606,8 +26957,11 @@
       <c r="BV116" s="4">
         <v>0</v>
       </c>
+      <c r="BW116" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="117" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>20</v>
       </c>
@@ -26830,8 +27184,11 @@
       <c r="BV117" s="4">
         <v>0</v>
       </c>
+      <c r="BW117" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="118" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>15</v>
       </c>
@@ -27054,8 +27411,11 @@
       <c r="BV118" s="4">
         <v>0</v>
       </c>
+      <c r="BW118" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="119" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>17</v>
       </c>
@@ -27278,8 +27638,11 @@
       <c r="BV119" s="4">
         <v>0</v>
       </c>
+      <c r="BW119" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="120" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>25</v>
       </c>
@@ -27502,8 +27865,11 @@
       <c r="BV120" s="4">
         <v>0</v>
       </c>
+      <c r="BW120" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="121" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>7</v>
       </c>
@@ -27726,8 +28092,11 @@
       <c r="BV121" s="4">
         <v>0</v>
       </c>
+      <c r="BW121" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="122" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>28</v>
       </c>
@@ -27950,8 +28319,11 @@
       <c r="BV122" s="4">
         <v>1</v>
       </c>
+      <c r="BW122" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="123" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>31</v>
       </c>
@@ -28174,8 +28546,11 @@
       <c r="BV123" s="4">
         <v>0</v>
       </c>
+      <c r="BW123" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="124" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>15</v>
       </c>
@@ -28398,8 +28773,11 @@
       <c r="BV124" s="4">
         <v>0</v>
       </c>
+      <c r="BW124" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="125" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>21</v>
       </c>
@@ -28622,8 +29000,11 @@
       <c r="BV125" s="4">
         <v>0</v>
       </c>
+      <c r="BW125" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="126" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>4</v>
       </c>
@@ -28846,8 +29227,11 @@
       <c r="BV126" s="4">
         <v>0</v>
       </c>
+      <c r="BW126" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="127" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>22</v>
       </c>
@@ -29070,8 +29454,11 @@
       <c r="BV127" s="4">
         <v>1</v>
       </c>
+      <c r="BW127" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="128" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>31</v>
       </c>
@@ -29294,8 +29681,11 @@
       <c r="BV128" s="4">
         <v>0</v>
       </c>
+      <c r="BW128" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="129" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>12</v>
       </c>
@@ -29518,8 +29908,11 @@
       <c r="BV129" s="4">
         <v>0</v>
       </c>
+      <c r="BW129" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="130" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>28</v>
       </c>
@@ -29742,8 +30135,11 @@
       <c r="BV130" s="4">
         <v>1</v>
       </c>
+      <c r="BW130" s="6">
+        <v>25</v>
+      </c>
     </row>
-    <row r="131" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>12</v>
       </c>
@@ -29966,8 +30362,11 @@
       <c r="BV131" s="4">
         <v>1</v>
       </c>
+      <c r="BW131" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="132" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>10</v>
       </c>
@@ -30190,8 +30589,11 @@
       <c r="BV132" s="4">
         <v>0</v>
       </c>
+      <c r="BW132" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="133" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>22</v>
       </c>
@@ -30414,8 +30816,11 @@
       <c r="BV133" s="4">
         <v>1</v>
       </c>
+      <c r="BW133" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="134" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>18</v>
       </c>
@@ -30638,8 +31043,11 @@
       <c r="BV134" s="4">
         <v>1</v>
       </c>
+      <c r="BW134" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="135" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>30</v>
       </c>
@@ -30862,8 +31270,11 @@
       <c r="BV135" s="4">
         <v>0</v>
       </c>
+      <c r="BW135" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="136" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>13</v>
       </c>
@@ -31086,8 +31497,11 @@
       <c r="BV136" s="4">
         <v>0</v>
       </c>
+      <c r="BW136" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="137" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>14</v>
       </c>
@@ -31310,8 +31724,11 @@
       <c r="BV137" s="4">
         <v>0</v>
       </c>
+      <c r="BW137" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="138" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>13</v>
       </c>
@@ -31534,8 +31951,11 @@
       <c r="BV138" s="4">
         <v>0</v>
       </c>
+      <c r="BW138" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="139" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>10</v>
       </c>
@@ -31758,8 +32178,11 @@
       <c r="BV139" s="4">
         <v>0</v>
       </c>
+      <c r="BW139" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="140" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>5</v>
       </c>
@@ -31982,8 +32405,11 @@
       <c r="BV140" s="4">
         <v>0</v>
       </c>
+      <c r="BW140" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="141" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>20</v>
       </c>
@@ -32206,8 +32632,11 @@
       <c r="BV141" s="4">
         <v>0</v>
       </c>
+      <c r="BW141" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="142" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>20</v>
       </c>
@@ -32430,8 +32859,11 @@
       <c r="BV142" s="4">
         <v>0</v>
       </c>
+      <c r="BW142" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="143" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>8</v>
       </c>
@@ -32654,8 +33086,11 @@
       <c r="BV143" s="4">
         <v>0</v>
       </c>
+      <c r="BW143" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="144" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>9</v>
       </c>
@@ -32878,8 +33313,11 @@
       <c r="BV144" s="4">
         <v>0</v>
       </c>
+      <c r="BW144" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="145" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>21</v>
       </c>
@@ -33102,8 +33540,11 @@
       <c r="BV145" s="4">
         <v>0</v>
       </c>
+      <c r="BW145" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="146" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>25.5</v>
       </c>
@@ -33326,8 +33767,11 @@
       <c r="BV146" s="4">
         <v>0</v>
       </c>
+      <c r="BW146" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="147" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>13</v>
       </c>
@@ -33550,8 +33994,11 @@
       <c r="BV147" s="4">
         <v>0</v>
       </c>
+      <c r="BW147" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="148" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>19</v>
       </c>
@@ -33774,8 +34221,11 @@
       <c r="BV148" s="4">
         <v>1</v>
       </c>
+      <c r="BW148" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="149" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>10</v>
       </c>
@@ -33998,8 +34448,11 @@
       <c r="BV149" s="4">
         <v>0</v>
       </c>
+      <c r="BW149" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="150" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>8</v>
       </c>
@@ -34222,8 +34675,11 @@
       <c r="BV150" s="4">
         <v>0</v>
       </c>
+      <c r="BW150" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="151" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>16</v>
       </c>
@@ -34446,8 +34902,11 @@
       <c r="BV151" s="4">
         <v>1</v>
       </c>
+      <c r="BW151" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="152" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>11</v>
       </c>
@@ -34670,8 +35129,11 @@
       <c r="BV152" s="4">
         <v>0</v>
       </c>
+      <c r="BW152" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="153" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>26</v>
       </c>
@@ -34894,8 +35356,11 @@
       <c r="BV153" s="4">
         <v>0</v>
       </c>
+      <c r="BW153" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="154" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>5</v>
       </c>
@@ -35118,8 +35583,11 @@
       <c r="BV154" s="4">
         <v>0</v>
       </c>
+      <c r="BW154" s="6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="155" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>9</v>
       </c>
@@ -35342,8 +35810,11 @@
       <c r="BV155" s="4">
         <v>0</v>
       </c>
+      <c r="BW155" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="156" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>16</v>
       </c>
@@ -35566,8 +36037,11 @@
       <c r="BV156" s="4">
         <v>1</v>
       </c>
+      <c r="BW156" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="157" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>22</v>
       </c>
@@ -35790,8 +36264,11 @@
       <c r="BV157" s="4">
         <v>0</v>
       </c>
+      <c r="BW157" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="158" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>22</v>
       </c>
@@ -36014,8 +36491,11 @@
       <c r="BV158" s="4">
         <v>0</v>
       </c>
+      <c r="BW158" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="159" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>15</v>
       </c>
@@ -36238,8 +36718,11 @@
       <c r="BV159" s="4">
         <v>1</v>
       </c>
+      <c r="BW159" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="160" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>20</v>
       </c>
@@ -36462,8 +36945,11 @@
       <c r="BV160" s="4">
         <v>1</v>
       </c>
+      <c r="BW160" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="161" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>13</v>
       </c>
@@ -36686,8 +37172,11 @@
       <c r="BV161" s="4">
         <v>0</v>
       </c>
+      <c r="BW161" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="162" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>13</v>
       </c>
@@ -36910,8 +37399,11 @@
       <c r="BV162" s="4">
         <v>0</v>
       </c>
+      <c r="BW162" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="163" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>19</v>
       </c>
@@ -37134,8 +37626,11 @@
       <c r="BV163" s="4">
         <v>0</v>
       </c>
+      <c r="BW163" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="164" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>13</v>
       </c>
@@ -37358,8 +37853,11 @@
       <c r="BV164" s="4">
         <v>0</v>
       </c>
+      <c r="BW164" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="165" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>13</v>
       </c>
@@ -37582,8 +38080,11 @@
       <c r="BV165" s="4">
         <v>0</v>
       </c>
+      <c r="BW165" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="166" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>14</v>
       </c>
@@ -37806,8 +38307,11 @@
       <c r="BV166" s="4">
         <v>0</v>
       </c>
+      <c r="BW166" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="167" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>8</v>
       </c>
@@ -38030,8 +38534,11 @@
       <c r="BV167" s="4">
         <v>0</v>
       </c>
+      <c r="BW167" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="168" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>20</v>
       </c>
@@ -38254,8 +38761,11 @@
       <c r="BV168" s="4">
         <v>0</v>
       </c>
+      <c r="BW168" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="169" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>21</v>
       </c>
@@ -38478,8 +38988,11 @@
       <c r="BV169" s="4">
         <v>0</v>
       </c>
+      <c r="BW169" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="170" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>21</v>
       </c>
@@ -38702,8 +39215,11 @@
       <c r="BV170" s="4">
         <v>0</v>
       </c>
+      <c r="BW170" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="171" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>6</v>
       </c>
@@ -38926,8 +39442,11 @@
       <c r="BV171" s="4">
         <v>0</v>
       </c>
+      <c r="BW171" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="172" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>30</v>
       </c>
@@ -39150,8 +39669,11 @@
       <c r="BV172" s="4">
         <v>0</v>
       </c>
+      <c r="BW172" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="173" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>17</v>
       </c>
@@ -39374,8 +39896,11 @@
       <c r="BV173" s="4">
         <v>0</v>
       </c>
+      <c r="BW173" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="174" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>13</v>
       </c>
@@ -39598,8 +40123,11 @@
       <c r="BV174" s="4">
         <v>0</v>
       </c>
+      <c r="BW174" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="175" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>31</v>
       </c>
@@ -39822,8 +40350,11 @@
       <c r="BV175" s="4">
         <v>0</v>
       </c>
+      <c r="BW175" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="176" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>10</v>
       </c>
@@ -40046,8 +40577,11 @@
       <c r="BV176" s="4">
         <v>0</v>
       </c>
+      <c r="BW176" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="177" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>12</v>
       </c>
@@ -40270,8 +40804,11 @@
       <c r="BV177" s="4">
         <v>1</v>
       </c>
+      <c r="BW177" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="178" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>16</v>
       </c>
@@ -40494,8 +41031,11 @@
       <c r="BV178" s="4">
         <v>0</v>
       </c>
+      <c r="BW178" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="179" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>5</v>
       </c>
@@ -40718,8 +41258,11 @@
       <c r="BV179" s="4">
         <v>0</v>
       </c>
+      <c r="BW179" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="180" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>14</v>
       </c>
@@ -40942,8 +41485,11 @@
       <c r="BV180" s="4">
         <v>0</v>
       </c>
+      <c r="BW180" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="181" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>18</v>
       </c>
@@ -41166,8 +41712,11 @@
       <c r="BV181" s="4">
         <v>0</v>
       </c>
+      <c r="BW181" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="182" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>27</v>
       </c>
@@ -41390,8 +41939,11 @@
       <c r="BV182" s="4">
         <v>1</v>
       </c>
+      <c r="BW182" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="183" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>32</v>
       </c>
@@ -41614,8 +42166,11 @@
       <c r="BV183" s="4">
         <v>1</v>
       </c>
+      <c r="BW183" s="6">
+        <v>28</v>
+      </c>
     </row>
-    <row r="184" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>13</v>
       </c>
@@ -41838,8 +42393,11 @@
       <c r="BV184" s="4">
         <v>0</v>
       </c>
+      <c r="BW184" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="185" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>36</v>
       </c>
@@ -42062,8 +42620,11 @@
       <c r="BV185" s="4">
         <v>0</v>
       </c>
+      <c r="BW185" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="186" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>10</v>
       </c>
@@ -42286,8 +42847,11 @@
       <c r="BV186" s="4">
         <v>0</v>
       </c>
+      <c r="BW186" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="187" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>8</v>
       </c>
@@ -42510,8 +43074,11 @@
       <c r="BV187" s="4">
         <v>0</v>
       </c>
+      <c r="BW187" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="188" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>26</v>
       </c>
@@ -42734,8 +43301,11 @@
       <c r="BV188" s="4">
         <v>0</v>
       </c>
+      <c r="BW188" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="189" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>33</v>
       </c>
@@ -42958,8 +43528,11 @@
       <c r="BV189" s="4">
         <v>1</v>
       </c>
+      <c r="BW189" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="190" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>29</v>
       </c>
@@ -43182,8 +43755,11 @@
       <c r="BV190" s="4">
         <v>1</v>
       </c>
+      <c r="BW190" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="191" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>8</v>
       </c>
@@ -43406,8 +43982,11 @@
       <c r="BV191" s="4">
         <v>0</v>
       </c>
+      <c r="BW191" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="192" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>17</v>
       </c>
@@ -43630,8 +44209,11 @@
       <c r="BV192" s="4">
         <v>1</v>
       </c>
+      <c r="BW192" s="6">
+        <v>27</v>
+      </c>
     </row>
-    <row r="193" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>22</v>
       </c>
@@ -43854,8 +44436,11 @@
       <c r="BV193" s="4">
         <v>0</v>
       </c>
+      <c r="BW193" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="194" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>11</v>
       </c>
@@ -44078,8 +44663,11 @@
       <c r="BV194" s="4">
         <v>1</v>
       </c>
+      <c r="BW194" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="195" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>20</v>
       </c>
@@ -44302,8 +44890,11 @@
       <c r="BV195" s="4">
         <v>0</v>
       </c>
+      <c r="BW195" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="196" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>26</v>
       </c>
@@ -44526,8 +45117,11 @@
       <c r="BV196" s="4">
         <v>0</v>
       </c>
+      <c r="BW196" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="197" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>20</v>
       </c>
@@ -44750,8 +45344,11 @@
       <c r="BV197" s="4">
         <v>0</v>
       </c>
+      <c r="BW197" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="198" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>21</v>
       </c>
@@ -44974,8 +45571,11 @@
       <c r="BV198" s="4">
         <v>0</v>
       </c>
+      <c r="BW198" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="199" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>24</v>
       </c>
@@ -45198,8 +45798,11 @@
       <c r="BV199" s="4">
         <v>0</v>
       </c>
+      <c r="BW199" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="200" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>36</v>
       </c>
@@ -45422,8 +46025,11 @@
       <c r="BV200" s="4">
         <v>1</v>
       </c>
+      <c r="BW200" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="201" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>21</v>
       </c>
@@ -45646,8 +46252,11 @@
       <c r="BV201" s="4">
         <v>0</v>
       </c>
+      <c r="BW201" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="202" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>8</v>
       </c>
@@ -45870,8 +46479,11 @@
       <c r="BV202" s="4">
         <v>0</v>
       </c>
+      <c r="BW202" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="203" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>6</v>
       </c>
@@ -46094,8 +46706,11 @@
       <c r="BV203" s="4">
         <v>0</v>
       </c>
+      <c r="BW203" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="204" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>14</v>
       </c>
@@ -46318,8 +46933,11 @@
       <c r="BV204" s="4">
         <v>0</v>
       </c>
+      <c r="BW204" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="205" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>15</v>
       </c>
@@ -46542,8 +47160,11 @@
       <c r="BV205" s="4">
         <v>1</v>
       </c>
+      <c r="BW205" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="206" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>23</v>
       </c>
@@ -46766,8 +47387,11 @@
       <c r="BV206" s="4">
         <v>1</v>
       </c>
+      <c r="BW206" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="207" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>34</v>
       </c>
@@ -46990,8 +47614,11 @@
       <c r="BV207" s="4">
         <v>1</v>
       </c>
+      <c r="BW207" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="208" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>14</v>
       </c>
@@ -47214,8 +47841,11 @@
       <c r="BV208" s="4">
         <v>0</v>
       </c>
+      <c r="BW208" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="209" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>29</v>
       </c>
@@ -47438,8 +48068,11 @@
       <c r="BV209" s="4">
         <v>1</v>
       </c>
+      <c r="BW209" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="210" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>14</v>
       </c>
@@ -47662,8 +48295,11 @@
       <c r="BV210" s="4">
         <v>0</v>
       </c>
+      <c r="BW210" s="6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="211" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>38</v>
       </c>
@@ -47886,8 +48522,11 @@
       <c r="BV211" s="4">
         <v>0</v>
       </c>
+      <c r="BW211" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="212" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>24</v>
       </c>
@@ -48110,8 +48749,11 @@
       <c r="BV212" s="4">
         <v>0</v>
       </c>
+      <c r="BW212" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="213" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>24</v>
       </c>
@@ -48334,8 +48976,11 @@
       <c r="BV213" s="4">
         <v>0</v>
       </c>
+      <c r="BW213" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="214" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>16</v>
       </c>
@@ -48558,8 +49203,11 @@
       <c r="BV214" s="4">
         <v>1</v>
       </c>
+      <c r="BW214" s="6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="215" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>20</v>
       </c>
@@ -48782,8 +49430,11 @@
       <c r="BV215" s="4">
         <v>0</v>
       </c>
+      <c r="BW215" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="216" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>7</v>
       </c>
@@ -49006,8 +49657,11 @@
       <c r="BV216" s="4">
         <v>0</v>
       </c>
+      <c r="BW216" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="217" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>36</v>
       </c>
@@ -49230,8 +49884,11 @@
       <c r="BV217" s="4">
         <v>1</v>
       </c>
+      <c r="BW217" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="218" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>22</v>
       </c>
@@ -49454,8 +50111,11 @@
       <c r="BV218" s="4">
         <v>0</v>
       </c>
+      <c r="BW218" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="219" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>18</v>
       </c>
@@ -49678,8 +50338,11 @@
       <c r="BV219" s="4">
         <v>0</v>
       </c>
+      <c r="BW219" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="220" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>4</v>
       </c>
@@ -49902,8 +50565,11 @@
       <c r="BV220" s="4">
         <v>0</v>
       </c>
+      <c r="BW220" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="221" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>30</v>
       </c>
@@ -50126,8 +50792,11 @@
       <c r="BV221" s="4">
         <v>0</v>
       </c>
+      <c r="BW221" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="222" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>32</v>
       </c>
@@ -50350,8 +51019,11 @@
       <c r="BV222" s="4">
         <v>1</v>
       </c>
+      <c r="BW222" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="223" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>11</v>
       </c>
@@ -50574,8 +51246,11 @@
       <c r="BV223" s="4">
         <v>1</v>
       </c>
+      <c r="BW223" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="224" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>25</v>
       </c>
@@ -50798,8 +51473,11 @@
       <c r="BV224" s="4">
         <v>0</v>
       </c>
+      <c r="BW224" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="225" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>11</v>
       </c>
@@ -51022,8 +51700,11 @@
       <c r="BV225" s="4">
         <v>0</v>
       </c>
+      <c r="BW225" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="226" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>11</v>
       </c>
@@ -51246,8 +51927,11 @@
       <c r="BV226" s="4">
         <v>0</v>
       </c>
+      <c r="BW226" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="227" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>13</v>
       </c>
@@ -51470,8 +52154,11 @@
       <c r="BV227" s="4">
         <v>0</v>
       </c>
+      <c r="BW227" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="228" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>17</v>
       </c>
@@ -51694,8 +52381,11 @@
       <c r="BV228" s="4">
         <v>0</v>
       </c>
+      <c r="BW228" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="229" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>19</v>
       </c>
@@ -51918,8 +52608,11 @@
       <c r="BV229" s="4">
         <v>0</v>
       </c>
+      <c r="BW229" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="230" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>11</v>
       </c>
@@ -52142,8 +52835,11 @@
       <c r="BV230" s="4">
         <v>1</v>
       </c>
+      <c r="BW230" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="231" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>22</v>
       </c>
@@ -52366,8 +53062,11 @@
       <c r="BV231" s="4">
         <v>0</v>
       </c>
+      <c r="BW231" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="232" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>26</v>
       </c>
@@ -52590,8 +53289,11 @@
       <c r="BV232" s="4">
         <v>0</v>
       </c>
+      <c r="BW232" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="233" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>17</v>
       </c>
@@ -52814,8 +53516,11 @@
       <c r="BV233" s="4">
         <v>0</v>
       </c>
+      <c r="BW233" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="234" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>22</v>
       </c>
@@ -53038,8 +53743,11 @@
       <c r="BV234" s="4">
         <v>0</v>
       </c>
+      <c r="BW234" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="235" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>37</v>
       </c>
@@ -53262,8 +53970,11 @@
       <c r="BV235" s="4">
         <v>0</v>
       </c>
+      <c r="BW235" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="236" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>17</v>
       </c>
@@ -53486,8 +54197,11 @@
       <c r="BV236" s="4">
         <v>0</v>
       </c>
+      <c r="BW236" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="237" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>10</v>
       </c>
@@ -53710,8 +54424,11 @@
       <c r="BV237" s="4">
         <v>0</v>
       </c>
+      <c r="BW237" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="238" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>15</v>
       </c>
@@ -53934,8 +54651,11 @@
       <c r="BV238" s="4">
         <v>1</v>
       </c>
+      <c r="BW238" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="239" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>36</v>
       </c>
@@ -54158,8 +54878,11 @@
       <c r="BV239" s="4">
         <v>0</v>
       </c>
+      <c r="BW239" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="240" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>9</v>
       </c>
@@ -54382,8 +55105,11 @@
       <c r="BV240" s="4">
         <v>0</v>
       </c>
+      <c r="BW240" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="241" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>24</v>
       </c>
@@ -54606,8 +55332,11 @@
       <c r="BV241" s="4">
         <v>1</v>
       </c>
+      <c r="BW241" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="242" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>12</v>
       </c>
@@ -54830,8 +55559,11 @@
       <c r="BV242" s="4">
         <v>0</v>
       </c>
+      <c r="BW242" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="243" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>18</v>
       </c>
@@ -55054,8 +55786,11 @@
       <c r="BV243" s="4">
         <v>0</v>
       </c>
+      <c r="BW243" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="244" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>15</v>
       </c>
@@ -55278,8 +56013,11 @@
       <c r="BV244" s="4">
         <v>1</v>
       </c>
+      <c r="BW244" s="6">
+        <v>29</v>
+      </c>
     </row>
-    <row r="245" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>32</v>
       </c>
@@ -55502,8 +56240,11 @@
       <c r="BV245" s="4">
         <v>1</v>
       </c>
+      <c r="BW245" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="246" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>22</v>
       </c>
@@ -55726,8 +56467,11 @@
       <c r="BV246" s="4">
         <v>1</v>
       </c>
+      <c r="BW246" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="247" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>31</v>
       </c>
@@ -55950,8 +56694,11 @@
       <c r="BV247" s="4">
         <v>0</v>
       </c>
+      <c r="BW247" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="248" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>4</v>
       </c>
@@ -56174,8 +56921,11 @@
       <c r="BV248" s="4">
         <v>0</v>
       </c>
+      <c r="BW248" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="249" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>16</v>
       </c>
@@ -56398,8 +57148,11 @@
       <c r="BV249" s="4">
         <v>0</v>
       </c>
+      <c r="BW249" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="250" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>31</v>
       </c>
@@ -56622,8 +57375,11 @@
       <c r="BV250" s="4">
         <v>1</v>
       </c>
+      <c r="BW250" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="251" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>27</v>
       </c>
@@ -56846,8 +57602,11 @@
       <c r="BV251" s="4">
         <v>1</v>
       </c>
+      <c r="BW251" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="252" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>26</v>
       </c>
@@ -57070,8 +57829,11 @@
       <c r="BV252" s="4">
         <v>1</v>
       </c>
+      <c r="BW252" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="253" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>17</v>
       </c>
@@ -57294,8 +58056,11 @@
       <c r="BV253" s="4">
         <v>0</v>
       </c>
+      <c r="BW253" s="6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="254" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>27</v>
       </c>
@@ -57518,8 +58283,11 @@
       <c r="BV254" s="4">
         <v>0</v>
       </c>
+      <c r="BW254" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="255" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>25</v>
       </c>
@@ -57742,8 +58510,11 @@
       <c r="BV255" s="4">
         <v>0</v>
       </c>
+      <c r="BW255" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="256" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>25</v>
       </c>
@@ -57966,8 +58737,11 @@
       <c r="BV256" s="4">
         <v>0</v>
       </c>
+      <c r="BW256" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="257" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>17</v>
       </c>
@@ -58190,8 +58964,11 @@
       <c r="BV257" s="4">
         <v>1</v>
       </c>
+      <c r="BW257" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="258" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>21</v>
       </c>
@@ -58414,8 +59191,11 @@
       <c r="BV258" s="4">
         <v>0</v>
       </c>
+      <c r="BW258" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="259" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>15</v>
       </c>
@@ -58638,8 +59418,11 @@
       <c r="BV259" s="4">
         <v>1</v>
       </c>
+      <c r="BW259" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="260" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>26</v>
       </c>
@@ -58862,8 +59645,11 @@
       <c r="BV260" s="4">
         <v>0</v>
       </c>
+      <c r="BW260" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="261" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>23</v>
       </c>
@@ -59086,8 +59872,11 @@
       <c r="BV261" s="4">
         <v>0</v>
       </c>
+      <c r="BW261" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="262" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>22</v>
       </c>
@@ -59310,8 +60099,11 @@
       <c r="BV262" s="4">
         <v>1</v>
       </c>
+      <c r="BW262" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="263" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>28</v>
       </c>
@@ -59534,8 +60326,11 @@
       <c r="BV263" s="4">
         <v>0</v>
       </c>
+      <c r="BW263" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="264" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>26</v>
       </c>
@@ -59758,8 +60553,11 @@
       <c r="BV264" s="4">
         <v>0</v>
       </c>
+      <c r="BW264" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="265" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>34</v>
       </c>
@@ -59982,8 +60780,11 @@
       <c r="BV265" s="4">
         <v>1</v>
       </c>
+      <c r="BW265" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="266" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>10</v>
       </c>
@@ -60206,8 +61007,11 @@
       <c r="BV266" s="4">
         <v>0</v>
       </c>
+      <c r="BW266" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="267" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>30</v>
       </c>
@@ -60430,8 +61234,11 @@
       <c r="BV267" s="4">
         <v>1</v>
       </c>
+      <c r="BW267" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="268" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>23</v>
       </c>
@@ -60654,8 +61461,11 @@
       <c r="BV268" s="4">
         <v>0</v>
       </c>
+      <c r="BW268" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="269" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>12</v>
       </c>
@@ -60878,8 +61688,11 @@
       <c r="BV269" s="4">
         <v>0</v>
       </c>
+      <c r="BW269" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="270" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>34</v>
       </c>
@@ -61102,8 +61915,11 @@
       <c r="BV270" s="4">
         <v>1</v>
       </c>
+      <c r="BW270" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="271" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>21</v>
       </c>
@@ -61326,8 +62142,11 @@
       <c r="BV271" s="4">
         <v>1</v>
       </c>
+      <c r="BW271" s="6">
+        <v>25</v>
+      </c>
     </row>
-    <row r="272" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>14</v>
       </c>
@@ -61550,8 +62369,11 @@
       <c r="BV272" s="4">
         <v>0</v>
       </c>
+      <c r="BW272" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="273" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>23</v>
       </c>
@@ -61774,8 +62596,11 @@
       <c r="BV273" s="4">
         <v>1</v>
       </c>
+      <c r="BW273" s="6">
+        <v>26</v>
+      </c>
     </row>
-    <row r="274" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>22</v>
       </c>
@@ -61998,8 +62823,11 @@
       <c r="BV274" s="4">
         <v>1</v>
       </c>
+      <c r="BW274" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="275" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>27</v>
       </c>
@@ -62222,8 +63050,11 @@
       <c r="BV275" s="4">
         <v>0</v>
       </c>
+      <c r="BW275" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="276" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>17</v>
       </c>
@@ -62446,8 +63277,11 @@
       <c r="BV276" s="4">
         <v>0</v>
       </c>
+      <c r="BW276" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="277" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>25</v>
       </c>
@@ -62670,8 +63504,11 @@
       <c r="BV277" s="4">
         <v>0</v>
       </c>
+      <c r="BW277" s="6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="278" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>33</v>
       </c>
@@ -62894,8 +63731,11 @@
       <c r="BV278" s="4">
         <v>1</v>
       </c>
+      <c r="BW278" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="279" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>14</v>
       </c>
@@ -63118,8 +63958,11 @@
       <c r="BV279" s="4">
         <v>0</v>
       </c>
+      <c r="BW279" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="280" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>20</v>
       </c>
@@ -63342,8 +64185,11 @@
       <c r="BV280" s="4">
         <v>0</v>
       </c>
+      <c r="BW280" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="281" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>9</v>
       </c>
@@ -63566,8 +64412,11 @@
       <c r="BV281" s="4">
         <v>1</v>
       </c>
+      <c r="BW281" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="282" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>20</v>
       </c>
@@ -63790,8 +64639,11 @@
       <c r="BV282" s="4">
         <v>0</v>
       </c>
+      <c r="BW282" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="283" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>25</v>
       </c>
@@ -64014,8 +64866,11 @@
       <c r="BV283" s="4">
         <v>1</v>
       </c>
+      <c r="BW283" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="284" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>11</v>
       </c>
@@ -64238,8 +65093,11 @@
       <c r="BV284" s="4">
         <v>1</v>
       </c>
+      <c r="BW284" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="285" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>31</v>
       </c>
@@ -64462,8 +65320,11 @@
       <c r="BV285" s="4">
         <v>1</v>
       </c>
+      <c r="BW285" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="286" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>13</v>
       </c>
@@ -64686,8 +65547,11 @@
       <c r="BV286" s="4">
         <v>1</v>
       </c>
+      <c r="BW286" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="287" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>36</v>
       </c>
@@ -64910,8 +65774,11 @@
       <c r="BV287" s="4">
         <v>0</v>
       </c>
+      <c r="BW287" s="6">
+        <v>28</v>
+      </c>
     </row>
-    <row r="288" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>14</v>
       </c>
@@ -65134,8 +66001,11 @@
       <c r="BV288" s="4">
         <v>1</v>
       </c>
+      <c r="BW288" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="289" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>32</v>
       </c>
@@ -65358,8 +66228,11 @@
       <c r="BV289" s="4">
         <v>0</v>
       </c>
+      <c r="BW289" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="290" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>16</v>
       </c>
@@ -65582,8 +66455,11 @@
       <c r="BV290" s="4">
         <v>0</v>
       </c>
+      <c r="BW290" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="291" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>41</v>
       </c>
@@ -65806,8 +66682,11 @@
       <c r="BV291" s="4">
         <v>0</v>
       </c>
+      <c r="BW291" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="292" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>7</v>
       </c>
@@ -66030,8 +66909,11 @@
       <c r="BV292" s="4">
         <v>1</v>
       </c>
+      <c r="BW292" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="293" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>27</v>
       </c>
@@ -66254,8 +67136,11 @@
       <c r="BV293" s="4">
         <v>0</v>
       </c>
+      <c r="BW293" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="294" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>14</v>
       </c>
@@ -66478,8 +67363,11 @@
       <c r="BV294" s="4">
         <v>0</v>
       </c>
+      <c r="BW294" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="295" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>24</v>
       </c>
@@ -66702,8 +67590,11 @@
       <c r="BV295" s="4">
         <v>0</v>
       </c>
+      <c r="BW295" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="296" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>26</v>
       </c>
@@ -66926,8 +67817,11 @@
       <c r="BV296" s="4">
         <v>1</v>
       </c>
+      <c r="BW296" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="297" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>16</v>
       </c>
@@ -67150,8 +68044,11 @@
       <c r="BV297" s="4">
         <v>0</v>
       </c>
+      <c r="BW297" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="298" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>21</v>
       </c>
@@ -67374,8 +68271,11 @@
       <c r="BV298" s="4">
         <v>0</v>
       </c>
+      <c r="BW298" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="299" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>46</v>
       </c>
@@ -67598,8 +68498,11 @@
       <c r="BV299" s="4">
         <v>0</v>
       </c>
+      <c r="BW299" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="300" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>14</v>
       </c>
@@ -67822,8 +68725,11 @@
       <c r="BV300" s="4">
         <v>1</v>
       </c>
+      <c r="BW300" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="301" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>12</v>
       </c>
@@ -68046,8 +68952,11 @@
       <c r="BV301" s="4">
         <v>1</v>
       </c>
+      <c r="BW301" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="302" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>22</v>
       </c>
@@ -68270,8 +69179,11 @@
       <c r="BV302" s="4">
         <v>0</v>
       </c>
+      <c r="BW302" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="303" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>22</v>
       </c>
@@ -68494,8 +69406,11 @@
       <c r="BV303" s="4">
         <v>1</v>
       </c>
+      <c r="BW303" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="304" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>22</v>
       </c>
@@ -68718,8 +69633,11 @@
       <c r="BV304" s="4">
         <v>1</v>
       </c>
+      <c r="BW304" s="6">
+        <v>21</v>
+      </c>
     </row>
-    <row r="305" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>14</v>
       </c>
@@ -68942,8 +69860,11 @@
       <c r="BV305" s="4">
         <v>1</v>
       </c>
+      <c r="BW305" s="6">
+        <v>6</v>
+      </c>
     </row>
-    <row r="306" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>21</v>
       </c>
@@ -69166,8 +70087,11 @@
       <c r="BV306" s="4">
         <v>1</v>
       </c>
+      <c r="BW306" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="307" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>8</v>
       </c>
@@ -69390,8 +70314,11 @@
       <c r="BV307" s="4">
         <v>1</v>
       </c>
+      <c r="BW307" s="6">
+        <v>9</v>
+      </c>
     </row>
-    <row r="308" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>7</v>
       </c>
@@ -69614,8 +70541,11 @@
       <c r="BV308" s="4">
         <v>0</v>
       </c>
+      <c r="BW308" s="6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="309" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>20</v>
       </c>
@@ -69838,8 +70768,11 @@
       <c r="BV309" s="4">
         <v>0</v>
       </c>
+      <c r="BW309" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="310" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>8</v>
       </c>
@@ -70062,8 +70995,11 @@
       <c r="BV310" s="4">
         <v>0</v>
       </c>
+      <c r="BW310" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="311" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>22</v>
       </c>
@@ -70286,8 +71222,11 @@
       <c r="BV311" s="4">
         <v>0</v>
       </c>
+      <c r="BW311" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="312" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>15</v>
       </c>
@@ -70510,8 +71449,11 @@
       <c r="BV312" s="4">
         <v>0</v>
       </c>
+      <c r="BW312" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="313" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>13</v>
       </c>
@@ -70734,8 +71676,11 @@
       <c r="BV313" s="4">
         <v>0</v>
       </c>
+      <c r="BW313" s="6">
+        <v>13</v>
+      </c>
     </row>
-    <row r="314" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>23</v>
       </c>
@@ -70958,8 +71903,11 @@
       <c r="BV314" s="4">
         <v>0</v>
       </c>
+      <c r="BW314" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="315" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>23</v>
       </c>
@@ -71182,8 +72130,11 @@
       <c r="BV315" s="4">
         <v>0</v>
       </c>
+      <c r="BW315" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="316" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>10</v>
       </c>
@@ -71406,8 +72357,11 @@
       <c r="BV316" s="4">
         <v>0</v>
       </c>
+      <c r="BW316" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="317" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>12</v>
       </c>
@@ -71630,8 +72584,11 @@
       <c r="BV317" s="4">
         <v>0</v>
       </c>
+      <c r="BW317" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="318" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>14</v>
       </c>
@@ -71854,8 +72811,11 @@
       <c r="BV318" s="4">
         <v>0</v>
       </c>
+      <c r="BW318" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="319" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>11</v>
       </c>
@@ -72078,8 +73038,11 @@
       <c r="BV319" s="4">
         <v>0</v>
       </c>
+      <c r="BW319" s="6">
+        <v>8</v>
+      </c>
     </row>
-    <row r="320" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>18</v>
       </c>
@@ -72302,8 +73265,11 @@
       <c r="BV320" s="4">
         <v>1</v>
       </c>
+      <c r="BW320" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="321" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>26</v>
       </c>
@@ -72526,8 +73492,11 @@
       <c r="BV321" s="4">
         <v>0</v>
       </c>
+      <c r="BW321" s="6">
+        <v>19</v>
+      </c>
     </row>
-    <row r="322" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>22</v>
       </c>
@@ -72750,8 +73719,11 @@
       <c r="BV322" s="4">
         <v>1</v>
       </c>
+      <c r="BW322" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="323" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>6</v>
       </c>
@@ -72974,8 +73946,11 @@
       <c r="BV323" s="4">
         <v>1</v>
       </c>
+      <c r="BW323" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="324" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>18</v>
       </c>
@@ -73198,8 +74173,11 @@
       <c r="BV324" s="4">
         <v>1</v>
       </c>
+      <c r="BW324" s="6">
+        <v>22</v>
+      </c>
     </row>
-    <row r="325" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>20</v>
       </c>
@@ -73422,8 +74400,11 @@
       <c r="BV325" s="4">
         <v>0</v>
       </c>
+      <c r="BW325" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="326" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>23</v>
       </c>
@@ -73646,8 +74627,11 @@
       <c r="BV326" s="4">
         <v>0</v>
       </c>
+      <c r="BW326" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="327" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>11</v>
       </c>
@@ -73870,8 +74854,11 @@
       <c r="BV327" s="4">
         <v>0</v>
       </c>
+      <c r="BW327" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="328" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>23</v>
       </c>
@@ -74094,8 +75081,11 @@
       <c r="BV328" s="4">
         <v>0</v>
       </c>
+      <c r="BW328" s="6">
+        <v>12</v>
+      </c>
     </row>
-    <row r="329" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>26</v>
       </c>
@@ -74318,8 +75308,11 @@
       <c r="BV329" s="4">
         <v>0</v>
       </c>
+      <c r="BW329" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="330" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>15</v>
       </c>
@@ -74542,8 +75535,11 @@
       <c r="BV330" s="4">
         <v>1</v>
       </c>
+      <c r="BW330" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="331" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>23</v>
       </c>
@@ -74766,8 +75762,11 @@
       <c r="BV331" s="4">
         <v>0</v>
       </c>
+      <c r="BW331" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="332" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>20</v>
       </c>
@@ -74990,8 +75989,11 @@
       <c r="BV332" s="4">
         <v>1</v>
       </c>
+      <c r="BW332" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="333" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>23</v>
       </c>
@@ -75214,8 +76216,11 @@
       <c r="BV333" s="4">
         <v>0</v>
       </c>
+      <c r="BW333" s="6">
+        <v>23</v>
+      </c>
     </row>
-    <row r="334" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>17</v>
       </c>
@@ -75438,8 +76443,11 @@
       <c r="BV334" s="4">
         <v>0</v>
       </c>
+      <c r="BW334" s="6">
+        <v>7</v>
+      </c>
     </row>
-    <row r="335" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>21</v>
       </c>
@@ -75662,8 +76670,11 @@
       <c r="BV335" s="4">
         <v>0</v>
       </c>
+      <c r="BW335" s="6">
+        <v>15</v>
+      </c>
     </row>
-    <row r="336" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>28</v>
       </c>
@@ -75886,8 +76897,11 @@
       <c r="BV336" s="4">
         <v>1</v>
       </c>
+      <c r="BW336" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="337" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>8</v>
       </c>
@@ -76110,8 +77124,11 @@
       <c r="BV337" s="4">
         <v>0</v>
       </c>
+      <c r="BW337" s="6">
+        <v>18</v>
+      </c>
     </row>
-    <row r="338" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>21</v>
       </c>
@@ -76334,8 +77351,11 @@
       <c r="BV338" s="4">
         <v>1</v>
       </c>
+      <c r="BW338" s="6">
+        <v>17</v>
+      </c>
     </row>
-    <row r="339" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>29</v>
       </c>
@@ -76558,8 +77578,11 @@
       <c r="BV339" s="4">
         <v>1</v>
       </c>
+      <c r="BW339" s="6">
+        <v>16</v>
+      </c>
     </row>
-    <row r="340" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>31</v>
       </c>
@@ -76782,8 +77805,11 @@
       <c r="BV340" s="4">
         <v>1</v>
       </c>
+      <c r="BW340" s="6">
+        <v>24</v>
+      </c>
     </row>
-    <row r="341" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>5</v>
       </c>
@@ -77006,8 +78032,11 @@
       <c r="BV341" s="4">
         <v>0</v>
       </c>
+      <c r="BW341" s="6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="342" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>11</v>
       </c>
@@ -77230,8 +78259,11 @@
       <c r="BV342" s="4">
         <v>0</v>
       </c>
+      <c r="BW342" s="6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="343" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>16</v>
       </c>
@@ -77454,8 +78486,11 @@
       <c r="BV343" s="4">
         <v>0</v>
       </c>
+      <c r="BW343" s="6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="344" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>16</v>
       </c>
@@ -77678,8 +78713,11 @@
       <c r="BV344" s="4">
         <v>0</v>
       </c>
+      <c r="BW344" s="6">
+        <v>14</v>
+      </c>
     </row>
-    <row r="345" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>19</v>
       </c>
@@ -77902,8 +78940,11 @@
       <c r="BV345" s="4">
         <v>1</v>
       </c>
+      <c r="BW345" s="6">
+        <v>20</v>
+      </c>
     </row>
-    <row r="346" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>27</v>
       </c>
@@ -78126,8 +79167,11 @@
       <c r="BV346" s="4">
         <v>0</v>
       </c>
+      <c r="BW346" s="6">
+        <v>10</v>
+      </c>
     </row>
-    <row r="347" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>24</v>
       </c>
@@ -78349,6 +79393,9 @@
       </c>
       <c r="BV347" s="4">
         <v>0</v>
+      </c>
+      <c r="BW347" s="6">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>